<commit_message>
Corrección de # y asignaciones
</commit_message>
<xml_diff>
--- a/out/production/compi/resources/matrizSintaxis.xlsx
+++ b/out/production/compi/resources/matrizSintaxis.xlsx
@@ -674,7 +674,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.000000"/>
       <color theme="1"/>
@@ -702,6 +702,11 @@
     </font>
     <font>
       <sz val="12.000000"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <color theme="1"/>
       <name val="Consolas"/>
     </font>
   </fonts>
@@ -761,7 +766,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -799,9 +804,7 @@
       <top style="thin">
         <color rgb="FFBF819E"/>
       </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -814,9 +817,7 @@
       <top style="thin">
         <color rgb="FFBF819E"/>
       </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -829,9 +830,7 @@
       <top style="thin">
         <color theme="1"/>
       </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -844,9 +843,7 @@
       <top style="thin">
         <color theme="1"/>
       </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -868,14 +865,27 @@
       <left style="thin">
         <color rgb="FF042E5D"/>
       </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF042E5D"/>
       </top>
       <bottom style="thin">
         <color rgb="FF042E5D"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="7" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="7" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -941,10 +951,10 @@
     <xf fontId="4" fillId="9" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="0">
+    <xf fontId="6" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="4" fillId="8" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0">
+    <xf fontId="4" fillId="8" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
@@ -1430,11 +1440,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="AZ1" zoomScale="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" ht="15.75">
       <c r="A1" s="1"/>
@@ -2643,7 +2654,7 @@
         <v>508</v>
       </c>
       <c r="U4" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V4" s="10">
         <v>508</v>
@@ -2796,7 +2807,7 @@
         <v>508</v>
       </c>
       <c r="BT4" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU4" s="10">
         <v>508</v>
@@ -3026,7 +3037,7 @@
         <v>506</v>
       </c>
       <c r="U5" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V5" s="10">
         <v>506</v>
@@ -3409,7 +3420,7 @@
         <v>508</v>
       </c>
       <c r="U6" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V6" s="10">
         <v>508</v>
@@ -3792,7 +3803,7 @@
         <v>508</v>
       </c>
       <c r="U7" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V7" s="10">
         <v>508</v>
@@ -4178,7 +4189,7 @@
         <v>508</v>
       </c>
       <c r="V8" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W8" s="10">
         <v>508</v>
@@ -4887,7 +4898,7 @@
         <v>133</v>
       </c>
       <c r="C10" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D10" s="10">
         <v>508</v>
@@ -5327,7 +5338,7 @@
         <v>509</v>
       </c>
       <c r="V11" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W11" s="10">
         <v>509</v>
@@ -6066,7 +6077,7 @@
         <v>510</v>
       </c>
       <c r="M13" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N13" s="10">
         <v>510</v>
@@ -6473,7 +6484,7 @@
         <v>511</v>
       </c>
       <c r="U14" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V14" s="10">
         <v>511</v>
@@ -6859,7 +6870,7 @@
         <v>508</v>
       </c>
       <c r="V15" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W15" s="10">
         <v>508</v>
@@ -7598,7 +7609,7 @@
         <v>510</v>
       </c>
       <c r="M17" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N17" s="10">
         <v>510</v>
@@ -8008,7 +8019,7 @@
         <v>508</v>
       </c>
       <c r="V18" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W18" s="10">
         <v>508</v>
@@ -8391,7 +8402,7 @@
         <v>508</v>
       </c>
       <c r="V19" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W19" s="10">
         <v>508</v>
@@ -10662,7 +10673,7 @@
         <v>510</v>
       </c>
       <c r="M25" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N25" s="10">
         <v>510</v>
@@ -11069,7 +11080,7 @@
         <v>511</v>
       </c>
       <c r="U26" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V26" s="10">
         <v>511</v>
@@ -11455,7 +11466,7 @@
         <v>508</v>
       </c>
       <c r="V27" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W27" s="10">
         <v>508</v>
@@ -11811,7 +11822,7 @@
         <v>510</v>
       </c>
       <c r="M28" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N28" s="10">
         <v>510</v>
@@ -12335,7 +12346,7 @@
         <v>520</v>
       </c>
       <c r="BH29" s="10">
-        <v>520</v>
+        <v>50</v>
       </c>
       <c r="BI29" s="10">
         <v>520</v>
@@ -12718,7 +12729,7 @@
         <v>521</v>
       </c>
       <c r="BH30" s="10">
-        <v>521</v>
+        <v>44</v>
       </c>
       <c r="BI30" s="10">
         <v>521</v>
@@ -13364,7 +13375,7 @@
         <v>523</v>
       </c>
       <c r="T32" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U32" s="10">
         <v>523</v>
@@ -13747,7 +13758,7 @@
         <v>510</v>
       </c>
       <c r="T33" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U33" s="10">
         <v>510</v>
@@ -14118,7 +14129,7 @@
         <v>514</v>
       </c>
       <c r="P34" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q34" s="10">
         <v>514</v>
@@ -14133,7 +14144,7 @@
         <v>514</v>
       </c>
       <c r="U34" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V34" s="10">
         <v>514</v>
@@ -14286,7 +14297,7 @@
         <v>514</v>
       </c>
       <c r="BT34" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU34" s="10">
         <v>514</v>
@@ -15118,10 +15129,10 @@
         <v>509</v>
       </c>
       <c r="CP36" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CQ36" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CR36" s="10">
         <v>509</v>
@@ -15228,7 +15239,7 @@
         <v>160</v>
       </c>
       <c r="C37" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D37" s="10">
         <v>510</v>
@@ -15668,7 +15679,7 @@
         <v>510</v>
       </c>
       <c r="V38" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W38" s="10">
         <v>510</v>
@@ -17033,10 +17044,10 @@
         <v>509</v>
       </c>
       <c r="CP41" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CQ41" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CR41" s="10">
         <v>509</v>
@@ -17143,7 +17154,7 @@
         <v>165</v>
       </c>
       <c r="C42" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D42" s="10">
         <v>510</v>
@@ -17583,7 +17594,7 @@
         <v>510</v>
       </c>
       <c r="V43" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W43" s="10">
         <v>510</v>
@@ -17984,7 +17995,7 @@
         <v>526</v>
       </c>
       <c r="AB44" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC44" s="10">
         <v>526</v>
@@ -18726,7 +18737,7 @@
         <v>523</v>
       </c>
       <c r="T46" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U46" s="10">
         <v>523</v>
@@ -19109,7 +19120,7 @@
         <v>510</v>
       </c>
       <c r="T47" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U47" s="10">
         <v>510</v>
@@ -20264,7 +20275,7 @@
         <v>508</v>
       </c>
       <c r="V50" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W50" s="10">
         <v>508</v>
@@ -21003,7 +21014,7 @@
         <v>510</v>
       </c>
       <c r="M52" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N52" s="10">
         <v>510</v>
@@ -21410,7 +21421,7 @@
         <v>511</v>
       </c>
       <c r="U53" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V53" s="10">
         <v>511</v>
@@ -21796,7 +21807,7 @@
         <v>508</v>
       </c>
       <c r="V54" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W54" s="10">
         <v>508</v>
@@ -23301,7 +23312,7 @@
         <v>510</v>
       </c>
       <c r="M58" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N58" s="10">
         <v>510</v>
@@ -23693,7 +23704,7 @@
         <v>530</v>
       </c>
       <c r="P59" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q59" s="10">
         <v>530</v>
@@ -23708,10 +23719,10 @@
         <v>530</v>
       </c>
       <c r="U59" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V59" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W59" s="10">
         <v>530</v>
@@ -23852,7 +23863,7 @@
         <v>530</v>
       </c>
       <c r="BQ59" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR59" s="10">
         <v>530</v>
@@ -23861,7 +23872,7 @@
         <v>530</v>
       </c>
       <c r="BT59" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU59" s="10">
         <v>530</v>
@@ -23912,7 +23923,7 @@
         <v>530</v>
       </c>
       <c r="CK59" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL59" s="10">
         <v>530</v>
@@ -24037,10 +24048,10 @@
         <v>183</v>
       </c>
       <c r="C60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E60" s="10">
         <v>531</v>
@@ -24064,7 +24075,7 @@
         <v>531</v>
       </c>
       <c r="L60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M60" s="10">
         <v>531</v>
@@ -24076,7 +24087,7 @@
         <v>531</v>
       </c>
       <c r="P60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q60" s="10">
         <v>531</v>
@@ -24091,13 +24102,13 @@
         <v>531</v>
       </c>
       <c r="U60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V60" s="10">
         <v>531</v>
       </c>
       <c r="W60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="X60" s="10">
         <v>531</v>
@@ -24142,7 +24153,7 @@
         <v>531</v>
       </c>
       <c r="AL60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AM60" s="10">
         <v>531</v>
@@ -24151,7 +24162,7 @@
         <v>531</v>
       </c>
       <c r="AO60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AP60" s="10">
         <v>531</v>
@@ -24172,10 +24183,10 @@
         <v>531</v>
       </c>
       <c r="AV60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AW60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AX60" s="10">
         <v>531</v>
@@ -24199,46 +24210,46 @@
         <v>531</v>
       </c>
       <c r="BE60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BF60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BG60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BH60" s="10">
         <v>531</v>
       </c>
       <c r="BI60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BJ60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BK60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BL60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BM60" s="10">
         <v>531</v>
       </c>
       <c r="BN60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BO60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BP60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BQ60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BS60" s="10">
         <v>531</v>
@@ -24268,34 +24279,34 @@
         <v>531</v>
       </c>
       <c r="CB60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CC60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CD60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CE60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CF60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CG60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CH60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CI60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CJ60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CK60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL60" s="10">
         <v>531</v>
@@ -24319,40 +24330,40 @@
         <v>531</v>
       </c>
       <c r="CS60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CT60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CU60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CV60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CW60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CX60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CY60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CZ60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DA60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DB60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DC60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DD60" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="DE60" s="10">
         <v>531</v>
@@ -24678,7 +24689,7 @@
         <v>508</v>
       </c>
       <c r="CK61" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL61" s="10">
         <v>508</v>
@@ -24860,7 +24871,7 @@
         <v>532</v>
       </c>
       <c r="V62" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W62" s="10">
         <v>532</v>
@@ -25444,7 +25455,7 @@
         <v>508</v>
       </c>
       <c r="CK63" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL63" s="10">
         <v>508</v>
@@ -25626,7 +25637,7 @@
         <v>508</v>
       </c>
       <c r="V64" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W64" s="10">
         <v>508</v>
@@ -26009,7 +26020,7 @@
         <v>508</v>
       </c>
       <c r="V65" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W65" s="10">
         <v>508</v>
@@ -26757,7 +26768,7 @@
         <v>510</v>
       </c>
       <c r="P67" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q67" s="10">
         <v>510</v>
@@ -27131,7 +27142,7 @@
         <v>510</v>
       </c>
       <c r="M68" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N68" s="10">
         <v>510</v>
@@ -28092,7 +28103,7 @@
         <v>528</v>
       </c>
       <c r="BZ70" s="10">
-        <v>528</v>
+        <v>182</v>
       </c>
       <c r="CA70" s="10">
         <v>528</v>
@@ -29450,7 +29461,7 @@
         <v>510</v>
       </c>
       <c r="T74" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U74" s="10">
         <v>510</v>
@@ -30171,22 +30182,22 @@
         <v>538</v>
       </c>
       <c r="E76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I76" s="10">
         <v>538</v>
       </c>
       <c r="J76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K76" s="10">
         <v>538</v>
@@ -30195,40 +30206,40 @@
         <v>538</v>
       </c>
       <c r="M76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N76" s="10">
         <v>538</v>
       </c>
       <c r="O76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S76" s="10">
         <v>538</v>
       </c>
       <c r="T76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W76" s="10">
         <v>538</v>
       </c>
       <c r="X76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y76" s="10">
         <v>538</v>
@@ -30240,31 +30251,31 @@
         <v>139</v>
       </c>
       <c r="AB76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD76" s="10">
         <v>538</v>
       </c>
       <c r="AE76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF76" s="10">
         <v>538</v>
       </c>
       <c r="AG76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI76" s="10">
         <v>538</v>
       </c>
       <c r="AJ76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK76" s="10">
         <v>538</v>
@@ -30273,7 +30284,7 @@
         <v>538</v>
       </c>
       <c r="AM76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN76" s="10">
         <v>538</v>
@@ -30282,16 +30293,16 @@
         <v>538</v>
       </c>
       <c r="AP76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AR76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AS76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT76" s="10">
         <v>538</v>
@@ -30306,16 +30317,16 @@
         <v>538</v>
       </c>
       <c r="AX76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AY76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ76" s="10">
         <v>538</v>
       </c>
       <c r="BA76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB76" s="10">
         <v>538</v>
@@ -30351,7 +30362,7 @@
         <v>538</v>
       </c>
       <c r="BM76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN76" s="10">
         <v>538</v>
@@ -30363,7 +30374,7 @@
         <v>538</v>
       </c>
       <c r="BQ76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR76" s="10">
         <v>538</v>
@@ -30372,7 +30383,7 @@
         <v>538</v>
       </c>
       <c r="BT76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU76" s="10">
         <v>538</v>
@@ -30423,7 +30434,7 @@
         <v>538</v>
       </c>
       <c r="CK76" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL76" s="10">
         <v>538</v>
@@ -30937,10 +30948,10 @@
         <v>539</v>
       </c>
       <c r="E78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G78" s="10">
         <v>143</v>
@@ -30952,7 +30963,7 @@
         <v>539</v>
       </c>
       <c r="J78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K78" s="10">
         <v>539</v>
@@ -30961,34 +30972,34 @@
         <v>539</v>
       </c>
       <c r="M78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N78" s="10">
         <v>539</v>
       </c>
       <c r="O78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S78" s="10">
         <v>539</v>
       </c>
       <c r="T78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W78" s="10">
         <v>539</v>
@@ -31000,37 +31011,37 @@
         <v>539</v>
       </c>
       <c r="Z78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AA78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD78" s="10">
         <v>539</v>
       </c>
       <c r="AE78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF78" s="10">
         <v>539</v>
       </c>
       <c r="AG78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI78" s="10">
         <v>539</v>
       </c>
       <c r="AJ78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK78" s="10">
         <v>539</v>
@@ -31039,7 +31050,7 @@
         <v>539</v>
       </c>
       <c r="AM78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN78" s="10">
         <v>539</v>
@@ -31048,16 +31059,16 @@
         <v>539</v>
       </c>
       <c r="AP78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AR78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AS78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT78" s="10">
         <v>539</v>
@@ -31072,16 +31083,16 @@
         <v>539</v>
       </c>
       <c r="AX78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AY78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ78" s="10">
         <v>539</v>
       </c>
       <c r="BA78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB78" s="10">
         <v>539</v>
@@ -31117,7 +31128,7 @@
         <v>539</v>
       </c>
       <c r="BM78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN78" s="10">
         <v>539</v>
@@ -31129,7 +31140,7 @@
         <v>539</v>
       </c>
       <c r="BQ78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR78" s="10">
         <v>539</v>
@@ -31138,7 +31149,7 @@
         <v>539</v>
       </c>
       <c r="BT78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU78" s="10">
         <v>539</v>
@@ -31189,7 +31200,7 @@
         <v>539</v>
       </c>
       <c r="CK78" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL78" s="10">
         <v>539</v>
@@ -31709,16 +31720,16 @@
         <v>153</v>
       </c>
       <c r="G80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I80" s="10">
         <v>540</v>
       </c>
       <c r="J80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K80" s="10">
         <v>540</v>
@@ -31727,55 +31738,55 @@
         <v>540</v>
       </c>
       <c r="M80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N80" s="10">
         <v>540</v>
       </c>
       <c r="O80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S80" s="10">
         <v>540</v>
       </c>
       <c r="T80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W80" s="10">
         <v>540</v>
       </c>
       <c r="X80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y80" s="10">
         <v>540</v>
       </c>
       <c r="Z80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AA80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB80" s="10">
         <v>146</v>
       </c>
       <c r="AC80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD80" s="10">
         <v>540</v>
@@ -31796,7 +31807,7 @@
         <v>540</v>
       </c>
       <c r="AJ80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK80" s="10">
         <v>540</v>
@@ -31805,7 +31816,7 @@
         <v>540</v>
       </c>
       <c r="AM80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN80" s="10">
         <v>540</v>
@@ -31817,13 +31828,13 @@
         <v>151</v>
       </c>
       <c r="AQ80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AR80" s="10">
         <v>150</v>
       </c>
       <c r="AS80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT80" s="10">
         <v>540</v>
@@ -31838,16 +31849,16 @@
         <v>540</v>
       </c>
       <c r="AX80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AY80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ80" s="10">
         <v>540</v>
       </c>
       <c r="BA80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB80" s="10">
         <v>540</v>
@@ -31883,7 +31894,7 @@
         <v>540</v>
       </c>
       <c r="BM80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN80" s="10">
         <v>540</v>
@@ -31895,7 +31906,7 @@
         <v>540</v>
       </c>
       <c r="BQ80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR80" s="10">
         <v>540</v>
@@ -31904,7 +31915,7 @@
         <v>540</v>
       </c>
       <c r="BT80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU80" s="10">
         <v>540</v>
@@ -31955,7 +31966,7 @@
         <v>540</v>
       </c>
       <c r="CK80" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL80" s="10">
         <v>540</v>
@@ -32469,22 +32480,22 @@
         <v>541</v>
       </c>
       <c r="E82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I82" s="10">
         <v>541</v>
       </c>
       <c r="J82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K82" s="10">
         <v>541</v>
@@ -32493,52 +32504,52 @@
         <v>541</v>
       </c>
       <c r="M82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N82" s="10">
         <v>541</v>
       </c>
       <c r="O82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S82" s="10">
         <v>541</v>
       </c>
       <c r="T82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W82" s="10">
         <v>541</v>
       </c>
       <c r="X82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y82" s="10">
         <v>541</v>
       </c>
       <c r="Z82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AA82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC82" s="10">
         <v>157</v>
@@ -32547,16 +32558,16 @@
         <v>541</v>
       </c>
       <c r="AE82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF82" s="10">
         <v>541</v>
       </c>
       <c r="AG82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI82" s="10">
         <v>541</v>
@@ -32580,13 +32591,13 @@
         <v>541</v>
       </c>
       <c r="AP82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ82" s="10">
         <v>158</v>
       </c>
       <c r="AR82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AS82" s="10">
         <v>159</v>
@@ -32604,16 +32615,16 @@
         <v>541</v>
       </c>
       <c r="AX82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AY82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ82" s="10">
         <v>541</v>
       </c>
       <c r="BA82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB82" s="10">
         <v>541</v>
@@ -32649,7 +32660,7 @@
         <v>541</v>
       </c>
       <c r="BM82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN82" s="10">
         <v>541</v>
@@ -32661,7 +32672,7 @@
         <v>541</v>
       </c>
       <c r="BQ82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR82" s="10">
         <v>541</v>
@@ -32670,7 +32681,7 @@
         <v>541</v>
       </c>
       <c r="BT82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU82" s="10">
         <v>541</v>
@@ -32721,7 +32732,7 @@
         <v>541</v>
       </c>
       <c r="CK82" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL82" s="10">
         <v>541</v>
@@ -33235,16 +33246,16 @@
         <v>542</v>
       </c>
       <c r="E84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I84" s="10">
         <v>542</v>
@@ -33259,76 +33270,76 @@
         <v>542</v>
       </c>
       <c r="M84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N84" s="10">
         <v>542</v>
       </c>
       <c r="O84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S84" s="10">
         <v>542</v>
       </c>
       <c r="T84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W84" s="10">
         <v>542</v>
       </c>
       <c r="X84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y84" s="10">
         <v>542</v>
       </c>
       <c r="Z84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AA84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD84" s="10">
         <v>542</v>
       </c>
       <c r="AE84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF84" s="10">
         <v>542</v>
       </c>
       <c r="AG84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI84" s="10">
         <v>542</v>
       </c>
       <c r="AJ84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK84" s="10">
         <v>542</v>
@@ -33337,7 +33348,7 @@
         <v>542</v>
       </c>
       <c r="AM84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN84" s="10">
         <v>542</v>
@@ -33346,16 +33357,16 @@
         <v>542</v>
       </c>
       <c r="AP84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AR84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AS84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT84" s="10">
         <v>542</v>
@@ -33373,7 +33384,7 @@
         <v>161</v>
       </c>
       <c r="AY84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ84" s="10">
         <v>542</v>
@@ -33415,7 +33426,7 @@
         <v>542</v>
       </c>
       <c r="BM84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN84" s="10">
         <v>542</v>
@@ -33427,7 +33438,7 @@
         <v>542</v>
       </c>
       <c r="BQ84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR84" s="10">
         <v>542</v>
@@ -33436,7 +33447,7 @@
         <v>542</v>
       </c>
       <c r="BT84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU84" s="10">
         <v>542</v>
@@ -33487,7 +33498,7 @@
         <v>542</v>
       </c>
       <c r="CK84" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL84" s="10">
         <v>542</v>
@@ -34001,22 +34012,22 @@
         <v>543</v>
       </c>
       <c r="E86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I86" s="10">
         <v>543</v>
       </c>
       <c r="J86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K86" s="10">
         <v>543</v>
@@ -34025,76 +34036,76 @@
         <v>543</v>
       </c>
       <c r="M86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N86" s="10">
         <v>543</v>
       </c>
       <c r="O86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S86" s="10">
         <v>543</v>
       </c>
       <c r="T86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W86" s="10">
         <v>543</v>
       </c>
       <c r="X86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y86" s="10">
         <v>543</v>
       </c>
       <c r="Z86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AA86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD86" s="10">
         <v>543</v>
       </c>
       <c r="AE86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF86" s="10">
         <v>543</v>
       </c>
       <c r="AG86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI86" s="10">
         <v>543</v>
       </c>
       <c r="AJ86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK86" s="10">
         <v>543</v>
@@ -34103,7 +34114,7 @@
         <v>543</v>
       </c>
       <c r="AM86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN86" s="10">
         <v>543</v>
@@ -34112,16 +34123,16 @@
         <v>543</v>
       </c>
       <c r="AP86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AR86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AS86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT86" s="10">
         <v>543</v>
@@ -34136,7 +34147,7 @@
         <v>543</v>
       </c>
       <c r="AX86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AY86" s="10">
         <v>165</v>
@@ -34145,7 +34156,7 @@
         <v>543</v>
       </c>
       <c r="BA86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB86" s="10">
         <v>543</v>
@@ -34181,7 +34192,7 @@
         <v>543</v>
       </c>
       <c r="BM86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN86" s="10">
         <v>543</v>
@@ -34193,7 +34204,7 @@
         <v>543</v>
       </c>
       <c r="BQ86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR86" s="10">
         <v>543</v>
@@ -34202,7 +34213,7 @@
         <v>543</v>
       </c>
       <c r="BT86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU86" s="10">
         <v>543</v>
@@ -34253,7 +34264,7 @@
         <v>543</v>
       </c>
       <c r="CK86" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL86" s="10">
         <v>543</v>
@@ -34761,7 +34772,7 @@
         <v>211</v>
       </c>
       <c r="C88" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D88" s="10">
         <v>545</v>
@@ -35150,22 +35161,22 @@
         <v>546</v>
       </c>
       <c r="E89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I89" s="10">
         <v>181</v>
       </c>
       <c r="J89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K89" s="10">
         <v>181</v>
@@ -35174,76 +35185,76 @@
         <v>173</v>
       </c>
       <c r="M89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N89" s="10">
         <v>546</v>
       </c>
       <c r="O89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S89" s="10">
         <v>172</v>
       </c>
       <c r="T89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W89" s="10">
         <v>546</v>
       </c>
       <c r="X89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y89" s="10">
         <v>181</v>
       </c>
       <c r="Z89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AA89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD89" s="10">
         <v>181</v>
       </c>
       <c r="AE89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF89" s="10">
         <v>181</v>
       </c>
       <c r="AG89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI89" s="10">
         <v>546</v>
       </c>
       <c r="AJ89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK89" s="10">
         <v>181</v>
@@ -35252,7 +35263,7 @@
         <v>546</v>
       </c>
       <c r="AM89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN89" s="10">
         <v>181</v>
@@ -35261,16 +35272,16 @@
         <v>546</v>
       </c>
       <c r="AP89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AR89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AS89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT89" s="10">
         <v>181</v>
@@ -35285,16 +35296,16 @@
         <v>546</v>
       </c>
       <c r="AX89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AY89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ89" s="10">
         <v>181</v>
       </c>
       <c r="BA89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB89" s="10">
         <v>181</v>
@@ -35330,7 +35341,7 @@
         <v>546</v>
       </c>
       <c r="BM89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN89" s="10">
         <v>546</v>
@@ -35342,7 +35353,7 @@
         <v>546</v>
       </c>
       <c r="BQ89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR89" s="10">
         <v>546</v>
@@ -35351,7 +35362,7 @@
         <v>546</v>
       </c>
       <c r="BT89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU89" s="10">
         <v>546</v>
@@ -35402,7 +35413,7 @@
         <v>546</v>
       </c>
       <c r="CK89" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL89" s="10">
         <v>546</v>
@@ -35533,22 +35544,22 @@
         <v>527</v>
       </c>
       <c r="E90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I90" s="10">
         <v>174</v>
       </c>
       <c r="J90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K90" s="10">
         <v>174</v>
@@ -35557,76 +35568,76 @@
         <v>527</v>
       </c>
       <c r="M90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N90" s="10">
         <v>527</v>
       </c>
       <c r="O90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S90" s="10">
         <v>527</v>
       </c>
       <c r="T90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W90" s="10">
         <v>527</v>
       </c>
       <c r="X90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y90" s="10">
         <v>174</v>
       </c>
       <c r="Z90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AA90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD90" s="10">
         <v>174</v>
       </c>
       <c r="AE90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF90" s="10">
         <v>174</v>
       </c>
       <c r="AG90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI90" s="10">
         <v>527</v>
       </c>
       <c r="AJ90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK90" s="10">
         <v>174</v>
@@ -35635,7 +35646,7 @@
         <v>527</v>
       </c>
       <c r="AM90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN90" s="10">
         <v>174</v>
@@ -35644,16 +35655,16 @@
         <v>527</v>
       </c>
       <c r="AP90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AR90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AS90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT90" s="10">
         <v>174</v>
@@ -35668,16 +35679,16 @@
         <v>527</v>
       </c>
       <c r="AX90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AY90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ90" s="10">
         <v>174</v>
       </c>
       <c r="BA90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB90" s="10">
         <v>174</v>
@@ -35713,7 +35724,7 @@
         <v>527</v>
       </c>
       <c r="BM90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN90" s="10">
         <v>527</v>
@@ -35725,7 +35736,7 @@
         <v>527</v>
       </c>
       <c r="BQ90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR90" s="10">
         <v>527</v>
@@ -35734,7 +35745,7 @@
         <v>527</v>
       </c>
       <c r="BT90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU90" s="10">
         <v>527</v>
@@ -35785,7 +35796,7 @@
         <v>527</v>
       </c>
       <c r="CK90" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL90" s="10">
         <v>527</v>
@@ -35916,22 +35927,22 @@
         <v>547</v>
       </c>
       <c r="E91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I91" s="10">
         <v>547</v>
       </c>
       <c r="J91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K91" s="10">
         <v>547</v>
@@ -35940,76 +35951,76 @@
         <v>547</v>
       </c>
       <c r="M91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N91" s="10">
         <v>547</v>
       </c>
       <c r="O91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Q91" s="10">
         <v>175</v>
       </c>
       <c r="R91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S91" s="10">
         <v>547</v>
       </c>
       <c r="T91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="V91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W91" s="10">
         <v>547</v>
       </c>
       <c r="X91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y91" s="10">
         <v>547</v>
       </c>
       <c r="Z91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AA91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AB91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD91" s="10">
         <v>547</v>
       </c>
       <c r="AE91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AF91" s="10">
         <v>547</v>
       </c>
       <c r="AG91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI91" s="10">
         <v>547</v>
       </c>
       <c r="AJ91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK91" s="10">
         <v>547</v>
@@ -36018,7 +36029,7 @@
         <v>547</v>
       </c>
       <c r="AM91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AN91" s="10">
         <v>547</v>
@@ -36027,16 +36038,16 @@
         <v>547</v>
       </c>
       <c r="AP91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AQ91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AR91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AS91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AT91" s="10">
         <v>547</v>
@@ -36051,16 +36062,16 @@
         <v>547</v>
       </c>
       <c r="AX91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AY91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AZ91" s="10">
         <v>547</v>
       </c>
       <c r="BA91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BB91" s="10">
         <v>547</v>
@@ -36096,7 +36107,7 @@
         <v>547</v>
       </c>
       <c r="BM91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BN91" s="10">
         <v>547</v>
@@ -36108,7 +36119,7 @@
         <v>547</v>
       </c>
       <c r="BQ91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BR91" s="10">
         <v>547</v>
@@ -36117,7 +36128,7 @@
         <v>547</v>
       </c>
       <c r="BT91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BU91" s="10">
         <v>547</v>
@@ -36168,7 +36179,7 @@
         <v>547</v>
       </c>
       <c r="CK91" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CL91" s="10">
         <v>547</v>
@@ -36323,7 +36334,7 @@
         <v>176</v>
       </c>
       <c r="M92" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N92" s="10">
         <v>523</v>
@@ -36706,7 +36717,7 @@
         <v>510</v>
       </c>
       <c r="M93" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N93" s="10">
         <v>510</v>
@@ -37086,7 +37097,7 @@
         <v>548</v>
       </c>
       <c r="L94" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M94" s="10">
         <v>548</v>
@@ -37443,7 +37454,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="10" aboveAverage="0" operator="greaterThan" rank="0" text="" id="{005E005A-00D3-44E8-BBAB-00D300730086}">
+          <x14:cfRule type="cellIs" priority="14" aboveAverage="0" operator="greaterThan" rank="0" text="" id="{00E90047-0001-4CF5-A2A4-009D00E500BE}">
             <xm:f>500</xm:f>
             <x14:dxf>
               <fill>
@@ -37457,7 +37468,7 @@
           <xm:sqref>A3:A94</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="9" aboveAverage="0" operator="equal" rank="0" text="" id="{00460024-00B3-4284-BA71-00BE00CF003D}">
+          <x14:cfRule type="cellIs" priority="13" aboveAverage="0" operator="equal" rank="0" text="" id="{00890004-0029-4C9A-BD23-007D00160092}">
             <xm:f>0</xm:f>
             <x14:dxf>
               <font>
@@ -37468,7 +37479,7 @@
           <xm:sqref>A3:A94</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="8" aboveAverage="0" operator="equal" rank="0" text="" id="{00550003-009C-4E88-B59C-00930083002D}">
+          <x14:cfRule type="cellIs" priority="12" aboveAverage="0" operator="equal" rank="0" text="" id="{00D80024-00A8-4989-81A0-00E4007C00A6}">
             <xm:f>180</xm:f>
             <x14:dxf>
               <fill>
@@ -37482,7 +37493,7 @@
           <xm:sqref>A3:A94</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" aboveAverage="0" operator="between" rank="0" text="" id="{008600CD-0074-4F7F-A07D-00B70099007E}">
+          <x14:cfRule type="cellIs" priority="11" aboveAverage="0" operator="between" rank="0" text="" id="{00500052-00C3-49D6-8D94-00D500EB0033}">
             <xm:f>1</xm:f>
             <xm:f>179</xm:f>
             <x14:dxf>
@@ -37497,7 +37508,7 @@
           <xm:sqref>A3:A94</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" aboveAverage="0" operator="greaterThan" rank="0" text="" id="{008A001D-0030-4695-9AD9-001400ED00BB}">
+          <x14:cfRule type="cellIs" priority="10" aboveAverage="0" operator="greaterThan" rank="0" text="" id="{005200ED-0086-41A6-8F1E-00C500BC0047}">
             <xm:f>600</xm:f>
             <x14:dxf>
               <fill>
@@ -37511,7 +37522,42 @@
           <xm:sqref>A3:A94</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="between" id="{004500D1-005C-4A1C-8D6C-009500B20054}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00A2008B-003E-43B6-AF7F-001F004A0041}">
+            <xm:f>183</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="-0.249977111117893"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFCBC0D9"/>
+                  <bgColor rgb="FFCBC0D9"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C2:DW94</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="between" id="{00E60074-0000-41D4-8D9C-00C100780058}">
+            <xm:f>0</xm:f>
+            <xm:f>183</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFC6EFCE"/>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C2:DW94</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="2" operator="between" id="{002A0022-0020-4D64-8880-007D00280015}">
             <xm:f>500</xm:f>
             <xm:f>599</xm:f>
             <x14:dxf>
@@ -37526,42 +37572,24 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C2:BG19 BI2:DW19 C20:DW21 C22:BG31 BI22:DW31 C32:DW32 C33:BG34 BI33:DW34 C35:DW35 C36:BG39 BI36:DW39 C40:DW40 C41:BG45 BI41:DW45 C46:DW46 C47:BG55 BI47:DW55 C56:DW56 C57:BG59 BI57:DW59 C60:DW60 C61:BG65 BI61:DW65 C66:DW66 C67:BG69 BI67:DW69 C70:DW70 C71:BG74 BI71:DW74 C75:DW75 C76:BG76 BI76:DW76 C77:DW77 C78:BG78 BI78:DW78 C79:DW79 C80:BG80 BI80:DW80 C81:DW81 C82:BG82 BI82:DW82 C83:DW83 C84:BG84 BI84:DW84 C85:DW85 C86:BG86 BI86:DW86 C87:DW87 C88:BG91 BI88:DW91 C92:DW92 C93:BG94 BI93:DW94 BH2:BH19 BH22:BH31 BH33:BH34 BH36:BH39 BH41:BH45 BH47:BH55 BH57:BH59 BH61:BH65 BH67:BH69 BH71:BH74 BH76 BH78 BH80 BH82 BH84 BH86 BH88:BH91 BH93:BH94</xm:sqref>
+          <xm:sqref>C2:DW94</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="between" id="{004E008D-0097-400B-9663-00AB00EB001E}">
-            <xm:f>0</xm:f>
-            <xm:f>181</xm:f>
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{005F00C8-00BA-47DD-99D8-009900C500D4}">
+            <xm:f>183</xm:f>
             <x14:dxf>
               <font>
-                <color rgb="FF006100"/>
+                <color theme="7" tint="-0.499984740745262"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFC6EFCE"/>
-                  <bgColor rgb="FFC6EFCE"/>
+                  <fgColor rgb="FFB2A1C6"/>
+                  <bgColor rgb="FFB2A1C6"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C2:BG19 BI2:DW19 C20:DW21 C22:BG31 BI22:DW31 C32:DW32 C33:BG34 BI33:DW34 C35:DW35 C36:BG39 BI36:DW39 C40:DW40 C41:BG45 BI41:DW45 C46:DW46 C47:BG55 BI47:DW55 C56:DW56 C57:BG59 BI57:DW59 C60:DW60 C61:BG65 BI61:DW65 C66:DW66 C67:BG69 BI67:DW69 C70:DW70 C71:BG74 BI71:DW74 C75:DW75 C76:BG76 BI76:DW76 C77:DW77 C78:BG78 BI78:DW78 C79:DW79 C80:BG80 BI80:DW80 C81:DW81 C82:BG82 BI82:DW82 C83:DW83 C84:BG84 BI84:DW84 C85:DW85 C86:BG86 BI86:DW86 C87:DW87 C88:BG91 BI88:DW91 C92:DW92 C93:BG94 BI93:DW94 BH2:BH19 BH22:BH31 BH33:BH34 BH36:BH39 BH41:BH45 BH47:BH55 BH57:BH59 BH61:BH65 BH67:BH69 BH71:BH74 BH76 BH78 BH80 BH82 BH84 BH86 BH88:BH91 BH93:BH94</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00730036-0014-487A-85E0-00CB00F200CE}">
-            <xm:f>182</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="-0.249977111117893"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFCBC0D9"/>
-                  <bgColor rgb="FFCBC0D9"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C2:BG19 BI2:DW19 C20:DW21 C22:BG31 BI22:DW31 C32:DW32 C33:BG34 BI33:DW34 C35:DW35 C36:BG39 BI36:DW39 C40:DW40 C41:BG45 BI41:DW45 C46:DW46 C47:BG55 BI47:DW55 C56:DW56 C57:BG59 BI57:DW59 C60:DW60 C61:BG65 BI61:DW65 C66:DW66 C67:BG69 BI67:DW69 C70:DW70 C71:BG74 BI71:DW74 C75:DW75 C76:BG76 BI76:DW76 C77:DW77 C78:BG78 BI78:DW78 C79:DW79 C80:BG80 BI80:DW80 C81:DW81 C82:BG82 BI82:DW82 C83:DW83 C84:BG84 BI84:DW84 C85:DW85 C86:BG86 BI86:DW86 C87:DW87 C88:BG91 BI88:DW91 C92:DW92 C93:BG94 BI93:DW94 BH2:BH19 BH22:BH31 BH33:BH34 BH36:BH39 BH41:BH45 BH47:BH55 BH57:BH59 BH61:BH65 BH67:BH69 BH71:BH74 BH76 BH78 BH80 BH82 BH84 BH86 BH88:BH91 BH93:BH94</xm:sqref>
+          <xm:sqref>C2:DW94</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>